<commit_message>
trinh | navigate to Category page from Homepage
</commit_message>
<xml_diff>
--- a/Automation/Demo/src/main/java/utils/TestData/UserData.xlsx
+++ b/Automation/Demo/src/main/java/utils/TestData/UserData.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="41">
   <si>
     <t>username</t>
   </si>
@@ -120,6 +120,36 @@
   </si>
   <si>
     <t>04012008</t>
+  </si>
+  <si>
+    <t>user73281@gmail.com</t>
+  </si>
+  <si>
+    <t>Aty9867@</t>
+  </si>
+  <si>
+    <t>zedwcfdg</t>
+  </si>
+  <si>
+    <t>0836159186</t>
+  </si>
+  <si>
+    <t>23121982</t>
+  </si>
+  <si>
+    <t>user98348@gmail.com</t>
+  </si>
+  <si>
+    <t>Aty8209@</t>
+  </si>
+  <si>
+    <t>ziyauxsi</t>
+  </si>
+  <si>
+    <t>0975392963</t>
+  </si>
+  <si>
+    <t>14121988</t>
   </si>
 </sst>
 </file>
@@ -186,7 +216,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -214,6 +244,42 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -550,23 +616,23 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="B2" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="C2" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="D2" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="E2" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="F2" s="16" t="s">
-        <v>30</v>
+      <c r="A2" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" s="24" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2" s="25" t="s">
+        <v>37</v>
+      </c>
+      <c r="E2" s="27" t="s">
+        <v>39</v>
+      </c>
+      <c r="F2" s="28" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">

</xml_diff>